<commit_message>
Refactored excel data reader
</commit_message>
<xml_diff>
--- a/src/main/java/Resources/CN_test_data.xlsx
+++ b/src/main/java/Resources/CN_test_data.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>deptCode</t>
   </si>
@@ -28,13 +27,37 @@
     <t>bookNumber</t>
   </si>
   <si>
-    <t>dept 1</t>
-  </si>
-  <si>
-    <t>FT1</t>
-  </si>
-  <si>
-    <t>BN1</t>
+    <t>Law</t>
+  </si>
+  <si>
+    <t>BP</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>numberOfbooks</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>bookletNature</t>
+  </si>
+  <si>
+    <t>numberOfPages</t>
+  </si>
+  <si>
+    <t>fromNumber</t>
+  </si>
+  <si>
+    <t>NAT</t>
+  </si>
+  <si>
+    <t>OPEN</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -70,8 +93,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -380,9 +404,10 @@
     <col min="4" max="4" width="17.85546875" customWidth="1"/>
     <col min="5" max="5" width="20.42578125" customWidth="1"/>
     <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -392,20 +417,51 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2">
         <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>